<commit_message>
Commit on morning of 06JUN2022
</commit_message>
<xml_diff>
--- a/(Example3) P51800032087/DUMP/rough.xlsx
+++ b/(Example3) P51800032087/DUMP/rough.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e291e7b128c337ee/Projects/Python/RERA/(Example3) P51800032087/DUMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{C3B09BA6-452A-4143-B1B5-EBECBB52EBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6187E07D-8130-47FF-BC89-FC2FF1FF0702}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="8_{C3B09BA6-452A-4143-B1B5-EBECBB52EBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72D3052E-090E-4005-A71C-7B90E306401D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BA283977-0174-4ABF-B5A4-87B2EB9E1EFD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Copy of the legal title report </t>
   </si>
@@ -116,6 +116,33 @@
   </si>
   <si>
     <t>20 Complaints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01 Copy of the legal title report </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02 Details of encumbrances </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 Copy of Layout Approval (in case of layout) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">04 Building Plan Approval / NA Order for plotted development </t>
+  </si>
+  <si>
+    <t xml:space="preserve">05 Commencement Certificates / NA Order for plotted development </t>
+  </si>
+  <si>
+    <t xml:space="preserve">06 Declaration about Commencement Certificate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">07 Declaration in FORM B </t>
+  </si>
+  <si>
+    <t>08 Architect’s Certificate of Percentage of Completion of Work (Form 1)</t>
+  </si>
+  <si>
+    <t>09 Engineer’s Certificate on Cost Incurred on Project (Form 2)</t>
   </si>
 </sst>
 </file>
@@ -491,12 +518,13 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -506,9 +534,8 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="str">
-        <f>CONCATENATE(A1," ",B1)</f>
-        <v xml:space="preserve">1 Copy of the legal title report </v>
+      <c r="D1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -518,9 +545,8 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="str">
-        <f t="shared" ref="D2:D19" si="0">CONCATENATE(A2," ",B2)</f>
-        <v xml:space="preserve">2 Details of encumbrances </v>
+      <c r="D2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,9 +556,8 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">3 Copy of Layout Approval (in case of layout) </v>
+      <c r="D3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -542,9 +567,8 @@
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">4 Building Plan Approval / NA Order for plotted development </v>
+      <c r="D4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -554,9 +578,8 @@
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">5 Commencement Certificates / NA Order for plotted development </v>
+      <c r="D5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -566,9 +589,8 @@
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">6 Declaration about Commencement Certificate </v>
+      <c r="D6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -578,9 +600,8 @@
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">7 Declaration in FORM B </v>
+      <c r="D7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,9 +611,8 @@
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>8 Architect’s Certificate of Percentage of Completion of Work (Form 1)</v>
+      <c r="D8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,9 +622,8 @@
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>9 Engineer’s Certificate on Cost Incurred on Project (Form 2)</v>
+      <c r="D9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -615,7 +634,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D2:D19" si="0">CONCATENATE(A10," ",B10)</f>
         <v xml:space="preserve">10 CERSAI details </v>
       </c>
     </row>

</xml_diff>